<commit_message>
add TC 08, 09, 10
</commit_message>
<xml_diff>
--- a/document/tcs (3).xlsx
+++ b/document/tcs (3).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -701,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:D51"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,7 +995,7 @@
       </c>
       <c r="D31" s="7"/>
     </row>
-    <row r="32" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">

</xml_diff>